<commit_message>
add new input into the documents
</commit_message>
<xml_diff>
--- a/Planning_IP-516vt_AppleTVApp4.xlsx
+++ b/Planning_IP-516vt_AppleTVApp4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27800" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="19540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Project Week</t>
   </si>
@@ -105,10 +105,37 @@
     <t>GUI</t>
   </si>
   <si>
-    <t>Anforderungsliste</t>
-  </si>
-  <si>
     <t>Bericht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live Stream Funkionalitäten </t>
+  </si>
+  <si>
+    <t>(Pausieren, Rück- und Vorspulen)</t>
+  </si>
+  <si>
+    <t>Video an Demand</t>
+  </si>
+  <si>
+    <t>TV Guide</t>
+  </si>
+  <si>
+    <t>Sendungsinformationen abrufen</t>
+  </si>
+  <si>
+    <t>verpasste Sendungen anschauen</t>
+  </si>
+  <si>
+    <t>Suchfunktion</t>
+  </si>
+  <si>
+    <t>Videos anschauen</t>
+  </si>
+  <si>
+    <t>Zusatzinformationen abrufen</t>
+  </si>
+  <si>
+    <t>Anbindung EPG</t>
   </si>
 </sst>
 </file>
@@ -118,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +183,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -203,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -499,8 +532,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -666,8 +787,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -728,20 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -760,59 +878,118 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="175">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -895,6 +1072,11 @@
     <cellStyle name="Besuchter Link" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -977,6 +1159,11 @@
     <cellStyle name="Link" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1255,7 +1442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1266,10 +1453,10 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E35" sqref="E35"/>
+      <selection pane="bottomRight" activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1280,27 +1467,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="31"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="60"/>
     </row>
     <row r="2" spans="1:23" ht="39" customHeight="1">
       <c r="A2" s="13"/>
@@ -1428,22 +1615,20 @@
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
-      <c r="J4" s="32"/>
+      <c r="J4" s="28"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23"/>
-      <c r="N4" s="32"/>
+      <c r="N4" s="28"/>
       <c r="O4" s="23"/>
       <c r="P4" s="23"/>
       <c r="Q4" s="23"/>
       <c r="R4" s="23"/>
       <c r="S4" s="24"/>
-      <c r="T4" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="82"/>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="6" t="s">
@@ -1457,15 +1642,15 @@
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="62"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
       <c r="O5" s="16"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="61"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
       <c r="S5" s="10"/>
     </row>
     <row r="6" spans="1:23">
@@ -1482,11 +1667,11 @@
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
-      <c r="L6" s="63"/>
+      <c r="L6" s="50"/>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
-      <c r="P6" s="63"/>
+      <c r="P6" s="50"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="S6" s="10"/>
@@ -1503,14 +1688,14 @@
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
-      <c r="L7" s="64"/>
+      <c r="L7" s="51"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
-      <c r="P7" s="65"/>
+      <c r="P7" s="52"/>
       <c r="Q7" s="19"/>
       <c r="R7" s="19"/>
-      <c r="S7" s="40"/>
+      <c r="S7" s="35"/>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" s="6" t="s">
@@ -1526,10 +1711,10 @@
       <c r="I8" s="16"/>
       <c r="J8" s="14"/>
       <c r="K8" s="19"/>
-      <c r="L8" s="65"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="19"/>
       <c r="N8" s="2"/>
-      <c r="P8" s="66"/>
+      <c r="P8" s="53"/>
       <c r="Q8" s="17"/>
       <c r="R8" s="15"/>
       <c r="S8" s="12"/>
@@ -1544,16 +1729,16 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
-      <c r="J9" s="46"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="46"/>
+      <c r="N9" s="40"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="50"/>
+      <c r="S9" s="43"/>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="8" t="s">
@@ -1568,11 +1753,9 @@
       <c r="H10" s="16"/>
       <c r="I10" s="18"/>
       <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="M10" s="18"/>
+      <c r="L10" s="18"/>
       <c r="N10" s="16"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="18"/>
+      <c r="P10" s="18"/>
       <c r="R10" s="16"/>
       <c r="S10" s="27"/>
     </row>
@@ -1590,7 +1773,7 @@
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="38"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -1617,8 +1800,8 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
       <c r="R12" s="3"/>
       <c r="S12" s="11"/>
     </row>
@@ -1626,10 +1809,10 @@
       <c r="A13" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="E13" s="28"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
@@ -1646,128 +1829,138 @@
       <c r="S13" s="24"/>
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="H14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34">
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="29">
         <v>16</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="32"/>
+      <c r="W15" s="32"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="51" t="s">
+      <c r="B16" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="34">
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="29">
         <v>14</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="37"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
+      <c r="H16" s="29"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="32"/>
+      <c r="W16" s="32"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="34">
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="29">
         <v>20</v>
       </c>
-      <c r="F17" s="34"/>
-      <c r="S17" s="41"/>
-      <c r="T17" s="37"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
+      <c r="H17" s="29"/>
+      <c r="S17" s="36"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="32"/>
+      <c r="W17" s="32"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="54"/>
-      <c r="B18" s="51" t="s">
+      <c r="A18" s="46"/>
+      <c r="B18" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="34">
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="29">
         <v>15</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
+      <c r="H18" s="29"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="32"/>
+      <c r="W18" s="32"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="42"/>
-      <c r="B19" s="51" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="34">
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="29">
         <v>5</v>
       </c>
-      <c r="F19" s="48"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="37"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
+      <c r="H19" s="41"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="32"/>
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="7" t="s">
@@ -1790,162 +1983,242 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="50"/>
-      <c r="T20" s="37"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-    </row>
-    <row r="21" spans="1:23" ht="30" customHeight="1">
-      <c r="B21" s="58" t="s">
+      <c r="S20" s="43"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="32"/>
+    </row>
+    <row r="21" spans="1:23" ht="15" customHeight="1">
+      <c r="B21" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="58"/>
-      <c r="D21" s="58"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="37"/>
-      <c r="U21" s="37"/>
-      <c r="V21" s="37"/>
-      <c r="W21" s="37"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="S21" s="36"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="32"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
     </row>
     <row r="22" spans="1:23" ht="30" customHeight="1">
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="37"/>
-      <c r="U22" s="37"/>
-      <c r="V22" s="37"/>
-      <c r="W22" s="37"/>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="B23" s="59" t="s">
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="S22" s="36"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+    </row>
+    <row r="23" spans="1:23" ht="15" customHeight="1">
+      <c r="B23" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="37"/>
-      <c r="U23" s="37"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-    </row>
-    <row r="24" spans="1:23">
-      <c r="B24" s="59" t="s">
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="S23" s="36"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="32"/>
+      <c r="W23" s="32"/>
+    </row>
+    <row r="24" spans="1:23" ht="15" customHeight="1">
+      <c r="B24" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-    </row>
-    <row r="25" spans="1:23">
-      <c r="B25" s="59" t="s">
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="32"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="32"/>
+      <c r="W24" s="32"/>
+    </row>
+    <row r="25" spans="1:23" ht="15" customHeight="1">
+      <c r="B25" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="37"/>
-      <c r="U25" s="37"/>
-      <c r="V25" s="37"/>
-      <c r="W25" s="37"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="S25" s="36"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="S26" s="41"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="S26" s="36"/>
     </row>
     <row r="27" spans="1:23">
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="S27" s="41"/>
-    </row>
-    <row r="28" spans="1:23">
-      <c r="A28" s="49" t="s">
+      <c r="A27" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="55"/>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="B29" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="47"/>
-      <c r="S29" s="41"/>
-    </row>
-    <row r="30" spans="1:23">
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="S30" s="41"/>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="S31" s="41"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="47"/>
+    </row>
+    <row r="28" spans="1:23" ht="30" customHeight="1">
+      <c r="A28" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="S28" s="36"/>
+    </row>
+    <row r="29" spans="1:23" ht="15" customHeight="1">
+      <c r="A29" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="S29" s="36"/>
+    </row>
+    <row r="30" spans="1:23" ht="30" customHeight="1">
+      <c r="B30" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="S30" s="36"/>
+    </row>
+    <row r="31" spans="1:23" ht="30" customHeight="1">
+      <c r="B31" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="S31" s="36"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="S32" s="41"/>
+      <c r="A32" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="S32" s="36"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56"/>
-      <c r="S33" s="41"/>
+      <c r="B33" s="64" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="S33" s="36"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="S34" s="41"/>
+      <c r="B34" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="S34" s="36"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
-      <c r="S35" s="41"/>
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="54"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="69"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="29"/>
+      <c r="S35" s="36"/>
     </row>
     <row r="36" spans="1:19">
-      <c r="A36" s="49" t="s">
+      <c r="A36" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
@@ -1958,62 +2231,63 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
-      <c r="S36" s="55"/>
+      <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="B37" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="S37" s="41"/>
+      <c r="B37" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="55"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="55"/>
+      <c r="S37" s="36"/>
     </row>
     <row r="38" spans="1:19">
-      <c r="S38" s="41"/>
+      <c r="S38" s="36"/>
     </row>
     <row r="39" spans="1:19">
-      <c r="S39" s="41"/>
+      <c r="S39" s="36"/>
     </row>
     <row r="40" spans="1:19">
-      <c r="S40" s="41"/>
+      <c r="S40" s="36"/>
     </row>
     <row r="41" spans="1:19">
-      <c r="S41" s="41"/>
+      <c r="S41" s="36"/>
     </row>
     <row r="42" spans="1:19">
-      <c r="S42" s="41"/>
+      <c r="S42" s="36"/>
     </row>
     <row r="43" spans="1:19">
-      <c r="S43" s="41"/>
+      <c r="S43" s="36"/>
     </row>
     <row r="44" spans="1:19">
-      <c r="S44" s="41"/>
+      <c r="S44" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B29:D29"/>
+  <mergeCells count="22">
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="T4:W4"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added more details. est. time planning through the semester
</commit_message>
<xml_diff>
--- a/Planning_IP-516vt_AppleTVApp4.xlsx
+++ b/Planning_IP-516vt_AppleTVApp4.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\IP-5_AppleTV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="19536" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>Project Week</t>
   </si>
@@ -69,9 +75,6 @@
     <t>Phase4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Phase2</t>
-  </si>
-  <si>
     <t>allg. Einarbeitung in die Materie</t>
   </si>
   <si>
@@ -90,9 +93,6 @@
     <t>Live Stream Implementation</t>
   </si>
   <si>
-    <t xml:space="preserve">analyse different Codes, Container </t>
-  </si>
-  <si>
     <t>DRM</t>
   </si>
   <si>
@@ -136,16 +136,123 @@
   </si>
   <si>
     <t>Anbindung EPG</t>
+  </si>
+  <si>
+    <t>Phase4 - Abschluss</t>
+  </si>
+  <si>
+    <t>Phase1 - Vorbereitung</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase2 - Vertiefung</t>
+  </si>
+  <si>
+    <t>Phase3 - Umsetzung</t>
+  </si>
+  <si>
+    <t>sum. Est.</t>
+  </si>
+  <si>
+    <t>sum. Real</t>
+  </si>
+  <si>
+    <t>Vertiefte Einarbeitung</t>
+  </si>
+  <si>
+    <t>Design-Entwurf</t>
+  </si>
+  <si>
+    <t>Analyse</t>
+  </si>
+  <si>
+    <t>Retroperspektive</t>
+  </si>
+  <si>
+    <t>Abschluss Bericht</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Milestone</t>
+  </si>
+  <si>
+    <t>Deliverys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufgabenvereinbarung
+</t>
+  </si>
+  <si>
+    <t>Funktionierende Entwicklungsumgebung</t>
+  </si>
+  <si>
+    <t>Eine erste Live-Stream-Implementation</t>
+  </si>
+  <si>
+    <t>Modulare Implementation erster Anf.</t>
+  </si>
+  <si>
+    <t>Erste Tutorial-Programme umgesetzt
+in TVML &amp; Swift</t>
+  </si>
+  <si>
+    <t>Erster Design-Prototyp als WireFrame</t>
+  </si>
+  <si>
+    <t>Auf usability getesteter Design-Prototyp V1</t>
+  </si>
+  <si>
+    <t>Funktionaler Prototyp V2</t>
+  </si>
+  <si>
+    <t>Auf usability getesteter Design-Prototyp V2</t>
+  </si>
+  <si>
+    <t>Phasendauer</t>
+  </si>
+  <si>
+    <t>Phasenaufwand</t>
+  </si>
+  <si>
+    <t>Wochen</t>
+  </si>
+  <si>
+    <t>Summe</t>
+  </si>
+  <si>
+    <t>Projektwoche</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analyse different Codecs, Container </t>
+  </si>
+  <si>
+    <t>Definition 5 verschiedener Streaming-Protokollen mit entsprechenden Containerformaten und codecs</t>
+  </si>
+  <si>
+    <t>Funktional getesteter Prototyp V1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +342,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="33">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -620,6 +739,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -798,7 +1005,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -905,178 +1112,205 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="175">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1442,7 +1676,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1452,42 +1686,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K45" sqref="K45"/>
+      <selection pane="bottomRight" activeCell="B24" sqref="B24:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="20" width="5.1640625" customWidth="1"/>
-    <col min="23" max="23" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="20" width="5.19921875" customWidth="1"/>
+    <col min="23" max="23" width="21.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="35" customHeight="1">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="34.950000000000003" customHeight="1">
+      <c r="A1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
-      <c r="S1" s="60"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="76"/>
     </row>
     <row r="2" spans="1:23" ht="39" customHeight="1">
       <c r="A2" s="13"/>
@@ -1546,7 +1780,7 @@
         <v>42385</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="16" thickBot="1">
+    <row r="3" spans="1:23" ht="16.2" thickBot="1">
       <c r="A3" s="9"/>
       <c r="B3" s="22">
         <v>38</v>
@@ -1603,7 +1837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="16" thickBot="1">
+    <row r="4" spans="1:23" ht="16.2" thickBot="1">
       <c r="A4" s="21" t="s">
         <v>4</v>
       </c>
@@ -1625,10 +1859,10 @@
       <c r="Q4" s="23"/>
       <c r="R4" s="23"/>
       <c r="S4" s="24"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="82"/>
-      <c r="W4" s="82"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="6" t="s">
@@ -1637,9 +1871,8 @@
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="49"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
       <c r="J5" s="48"/>
@@ -1660,8 +1893,8 @@
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
       <c r="D6" s="16"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="51"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
@@ -1683,9 +1916,8 @@
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="50"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16"/>
       <c r="L7" s="51"/>
@@ -1704,9 +1936,8 @@
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="52"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="14"/>
@@ -1747,17 +1978,23 @@
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="18"/>
       <c r="J10" s="19"/>
-      <c r="L10" s="18"/>
+      <c r="K10" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="N10" s="16"/>
-      <c r="P10" s="18"/>
+      <c r="O10" s="18" t="s">
+        <v>50</v>
+      </c>
       <c r="R10" s="16"/>
-      <c r="S10" s="27"/>
+      <c r="S10" s="27" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" s="6" t="s">
@@ -1782,7 +2019,7 @@
       <c r="R11" s="16"/>
       <c r="S11" s="10"/>
     </row>
-    <row r="12" spans="1:23" ht="16" thickBot="1">
+    <row r="12" spans="1:23" ht="16.2" thickBot="1">
       <c r="A12" s="7" t="s">
         <v>1</v>
       </c>
@@ -1805,7 +2042,7 @@
       <c r="R12" s="3"/>
       <c r="S12" s="11"/>
     </row>
-    <row r="13" spans="1:23" ht="16" thickBot="1">
+    <row r="13" spans="1:23" ht="16.2" thickBot="1">
       <c r="A13" s="21" t="s">
         <v>5</v>
       </c>
@@ -1830,29 +2067,37 @@
     </row>
     <row r="14" spans="1:23" ht="30" customHeight="1">
       <c r="A14" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="66"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="38" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
+      <c r="I14" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="85" t="s">
+        <v>42</v>
+      </c>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
+      <c r="M14" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
+      <c r="P14" s="30" t="s">
+        <v>64</v>
+      </c>
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="39"/>
@@ -1863,19 +2108,39 @@
     </row>
     <row r="15" spans="1:23">
       <c r="A15" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="70" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="71"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="29">
         <v>16</v>
       </c>
-      <c r="H15" s="37"/>
+      <c r="H15" s="37">
+        <v>14</v>
+      </c>
+      <c r="I15">
+        <f>SUM(G15:G19)</f>
+        <v>76</v>
+      </c>
+      <c r="J15">
+        <f>SUM(H15:H19)</f>
+        <v>70</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15" t="s">
+        <v>65</v>
+      </c>
+      <c r="P15">
+        <f>M15*10*2</f>
+        <v>80</v>
+      </c>
       <c r="S15" s="36"/>
       <c r="T15" s="32"/>
       <c r="U15" s="32"/>
@@ -1884,19 +2149,21 @@
     </row>
     <row r="16" spans="1:23">
       <c r="A16" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="66"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="29">
         <v>18</v>
       </c>
-      <c r="B16" s="72" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73"/>
-      <c r="E16" s="73"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="29">
-        <v>14</v>
-      </c>
-      <c r="H16" s="29"/>
+      <c r="H16" s="29">
+        <v>12</v>
+      </c>
       <c r="S16" s="36"/>
       <c r="T16" s="32"/>
       <c r="U16" s="32"/>
@@ -1905,19 +2172,21 @@
     </row>
     <row r="17" spans="1:23">
       <c r="A17" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="29">
         <v>20</v>
       </c>
-      <c r="H17" s="29"/>
+      <c r="H17" s="29">
+        <v>22</v>
+      </c>
       <c r="S17" s="36"/>
       <c r="T17" s="32"/>
       <c r="U17" s="32"/>
@@ -1926,17 +2195,19 @@
     </row>
     <row r="18" spans="1:23">
       <c r="A18" s="46"/>
-      <c r="B18" s="72" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="73"/>
-      <c r="E18" s="73"/>
-      <c r="F18" s="74"/>
+      <c r="B18" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="29">
-        <v>15</v>
-      </c>
-      <c r="H18" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="H18" s="29">
+        <v>16</v>
+      </c>
       <c r="S18" s="36"/>
       <c r="T18" s="32"/>
       <c r="U18" s="32"/>
@@ -1945,17 +2216,19 @@
     </row>
     <row r="19" spans="1:23">
       <c r="A19" s="37"/>
-      <c r="B19" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="77"/>
+      <c r="B19" s="68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
       <c r="G19" s="29">
-        <v>5</v>
-      </c>
-      <c r="H19" s="41"/>
+        <v>8</v>
+      </c>
+      <c r="H19" s="41">
+        <v>6</v>
+      </c>
       <c r="S19" s="36"/>
       <c r="T19" s="32"/>
       <c r="U19" s="32"/>
@@ -1964,7 +2237,7 @@
     </row>
     <row r="20" spans="1:23">
       <c r="A20" s="7" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1977,10 +2250,14 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="M20" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="P20" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="43"/>
@@ -1990,15 +2267,28 @@
       <c r="W20" s="32"/>
     </row>
     <row r="21" spans="1:23" ht="15" customHeight="1">
-      <c r="B21" s="61" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
+      <c r="A21" s="45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="71" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
       <c r="G21" s="29"/>
       <c r="H21" s="29"/>
+      <c r="M21">
+        <v>6</v>
+      </c>
+      <c r="N21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P21">
+        <f>M21*10*2</f>
+        <v>120</v>
+      </c>
       <c r="S21" s="36"/>
       <c r="T21" s="32"/>
       <c r="U21" s="32"/>
@@ -2006,13 +2296,16 @@
       <c r="W21" s="32"/>
     </row>
     <row r="22" spans="1:23" ht="30" customHeight="1">
-      <c r="B22" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
+      <c r="A22" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="72" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="S22" s="36"/>
@@ -2022,13 +2315,16 @@
       <c r="W22" s="32"/>
     </row>
     <row r="23" spans="1:23" ht="15" customHeight="1">
-      <c r="B23" s="56" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
+      <c r="A23" s="96" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="72" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
       <c r="S23" s="36"/>
@@ -2038,13 +2334,13 @@
       <c r="W23" s="32"/>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1">
-      <c r="B24" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
+      <c r="B24" s="72" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
       <c r="S24" s="36"/>
@@ -2054,13 +2350,13 @@
       <c r="W24" s="32"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1">
-      <c r="B25" s="56" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
+      <c r="B25" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
       <c r="S25" s="36"/>
@@ -2070,20 +2366,20 @@
       <c r="W25" s="32"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="B26" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
+      <c r="B26" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
       <c r="S26" s="36"/>
     </row>
     <row r="27" spans="1:23">
       <c r="A27" s="42" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2096,123 +2392,158 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
+      <c r="M27" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
+      <c r="P27" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
       <c r="S27" s="47"/>
     </row>
     <row r="28" spans="1:23" ht="30" customHeight="1">
-      <c r="A28" s="63" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
+      <c r="A28" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
+      <c r="M28" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29">
+        <v>40</v>
+      </c>
       <c r="S28" s="36"/>
     </row>
     <row r="29" spans="1:23" ht="15" customHeight="1">
-      <c r="A29" s="65" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="74"/>
+      <c r="A29" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="77" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="67"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
+      <c r="L29" s="101" t="s">
+        <v>68</v>
+      </c>
+      <c r="M29" s="29">
+        <v>3</v>
+      </c>
+      <c r="N29" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29">
+        <f>SUM(M29*10*2)</f>
+        <v>60</v>
+      </c>
       <c r="S29" s="36"/>
     </row>
     <row r="30" spans="1:23" ht="30" customHeight="1">
-      <c r="B30" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
+      <c r="B30" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="82"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
+      <c r="M30" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29">
+        <f>SUM(P28:P29)</f>
+        <v>100</v>
+      </c>
       <c r="S30" s="36"/>
     </row>
     <row r="31" spans="1:23" ht="30" customHeight="1">
-      <c r="B31" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
+      <c r="B31" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="82"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="82"/>
+      <c r="F31" s="82"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
       <c r="S31" s="36"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="A32" s="78" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="64" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="80"/>
+      <c r="A32" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="83"/>
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
       <c r="S32" s="36"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="B33" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="80"/>
+      <c r="B33" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="83"/>
       <c r="G33" s="29"/>
       <c r="H33" s="29"/>
       <c r="S33" s="36"/>
     </row>
     <row r="34" spans="1:19">
       <c r="B34" s="84" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C34" s="84"/>
       <c r="D34" s="84"/>
       <c r="E34" s="84"/>
-      <c r="F34" s="80"/>
+      <c r="F34" s="83"/>
       <c r="G34" s="29"/>
       <c r="H34" s="29"/>
       <c r="S34" s="36"/>
     </row>
     <row r="35" spans="1:19">
       <c r="A35" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="83"/>
+        <v>36</v>
+      </c>
+      <c r="B35" s="78"/>
+      <c r="C35" s="78"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="61"/>
       <c r="H35" s="29"/>
       <c r="S35" s="36"/>
     </row>
     <row r="36" spans="1:19">
       <c r="A36" s="42" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
@@ -2225,28 +2556,62 @@
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
+      <c r="M36" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="P36" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="47"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="B37" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
+      <c r="B37" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37" t="s">
+        <v>65</v>
+      </c>
+      <c r="P37">
+        <f>M37*10*2</f>
+        <v>40</v>
+      </c>
       <c r="S37" s="36"/>
     </row>
     <row r="38" spans="1:19">
+      <c r="B38" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
       <c r="S38" s="36"/>
     </row>
     <row r="39" spans="1:19">
+      <c r="B39" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
       <c r="S39" s="36"/>
     </row>
     <row r="40" spans="1:19">
@@ -2265,29 +2630,31 @@
       <c r="S44" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
+  <mergeCells count="24">
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="B26:F26"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2297,4 +2664,119 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="23.296875" customWidth="1"/>
+    <col min="2" max="2" width="36.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="31.2">
+      <c r="A2" s="99" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="31.2">
+      <c r="A3" s="88"/>
+      <c r="B3" s="89" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="31.8" thickBot="1">
+      <c r="A4" s="90"/>
+      <c r="B4" s="91" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="31.2">
+      <c r="A5" s="100" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="92" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="88"/>
+      <c r="B6" s="93" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="47.4" thickBot="1">
+      <c r="A7" s="90"/>
+      <c r="B7" s="91" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="100" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="95" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="88"/>
+      <c r="B9" s="93" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="88"/>
+      <c r="B10" s="93"/>
+    </row>
+    <row r="11" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A11" s="97"/>
+      <c r="B11" s="98"/>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="100" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="95" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="31.2">
+      <c r="A13" s="88"/>
+      <c r="B13" s="89" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="88"/>
+      <c r="B14" s="93" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16.2" thickBot="1">
+      <c r="A15" s="90"/>
+      <c r="B15" s="94" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>